<commit_message>
affix progress bar clean up item getting/rendering/displaying logic a little (still unhappy with it)
</commit_message>
<xml_diff>
--- a/documentation/Example files/test_skipifs.xlsx
+++ b/documentation/Example files/test_skipifs.xlsx
@@ -19,55 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="77">
-  <si>
-    <t>typ</t>
-  </si>
-  <si>
-    <t>variablenname</t>
-  </si>
-  <si>
-    <t>wortlaut</t>
-  </si>
-  <si>
-    <t>MCalt1</t>
-  </si>
-  <si>
-    <t>MCalt2</t>
-  </si>
-  <si>
-    <t>MCalt3</t>
-  </si>
-  <si>
-    <t>MCalt4</t>
-  </si>
-  <si>
-    <t>MCalt5</t>
-  </si>
-  <si>
-    <t>MCalt6</t>
-  </si>
-  <si>
-    <t>MCalt7</t>
-  </si>
-  <si>
-    <t>MCalt8</t>
-  </si>
-  <si>
-    <t>MCalt9</t>
-  </si>
-  <si>
-    <t>MCalt10</t>
-  </si>
-  <si>
-    <t>MCalt11</t>
-  </si>
-  <si>
-    <t>MCalt12</t>
-  </si>
-  <si>
-    <t>instruction</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t>mc</t>
   </si>
@@ -136,19 +88,10 @@
     <t>dont show mc2</t>
   </si>
   <si>
-    <t>skipif</t>
-  </si>
-  <si>
-    <t>mc1 != 1</t>
-  </si>
-  <si>
     <t>show mc3</t>
   </si>
   <si>
     <t>dont show mc3</t>
-  </si>
-  <si>
-    <t>mc2 != 1</t>
   </si>
   <si>
     <t>mc3</t>
@@ -168,9 +111,6 @@
   </si>
   <si>
     <t>offen1</t>
-  </si>
-  <si>
-    <t>offen 4</t>
   </si>
   <si>
     <t>mc4</t>
@@ -233,9 +173,6 @@
 shown only if 'xxx' typed into offen before</t>
   </si>
   <si>
-    <t>alter &lt; 18</t>
-  </si>
-  <si>
     <t>enter age gte 18 to show alcohol question  
 Displayed if MC3 and MC4 both have the second option selected.</t>
   </si>
@@ -246,16 +183,55 @@
     <t>pu</t>
   </si>
   <si>
-    <t>mc1 = 2 &amp;&amp; mc2 = 2</t>
-  </si>
-  <si>
-    <t>mc3 != 1 &amp;&amp; mc4 != 2</t>
-  </si>
-  <si>
-    <t>mc3 = 1 || mc4 = 1</t>
-  </si>
-  <si>
-    <t>people == 'Klara, Heinz'</t>
+    <t>note</t>
+  </si>
+  <si>
+    <t>text 4</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>choice1</t>
+  </si>
+  <si>
+    <t>choice2</t>
+  </si>
+  <si>
+    <t>choice3</t>
+  </si>
+  <si>
+    <t>choice4</t>
+  </si>
+  <si>
+    <t>showif</t>
+  </si>
+  <si>
+    <t>people %contains% 2</t>
+  </si>
+  <si>
+    <t>alter &gt; 18</t>
+  </si>
+  <si>
+    <t>mc3 == 2 &amp;&amp; mc4 == 2</t>
+  </si>
+  <si>
+    <t>mc3 == 1 || mc4 == 2</t>
+  </si>
+  <si>
+    <t>mc1 == 1 &amp;&amp; mc2 == 1</t>
+  </si>
+  <si>
+    <t>mc2 == 1</t>
+  </si>
+  <si>
+    <t>mc1 == 1</t>
   </si>
 </sst>
 </file>
@@ -640,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -658,299 +634,275 @@
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="18">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="18">
       <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="D2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30">
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30">
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45">
+      <c r="B10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="B12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="I13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="B15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="E15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="I15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="J15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="30">
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="30">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="30">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="30">
-      <c r="A7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="45">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="30">
-      <c r="B9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="45">
-      <c r="B10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="B12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="D14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="30">
-      <c r="B15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
     </row>

</xml_diff>